<commit_message>
data dictionary minor update
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v4.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beto\OneDrive\UNICEF\TransMonEE\data-etl\tmee\data_in\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_0ED489CFCE2D5BBE6E7F372033D5229152D9D0AC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0CCF4BB-681D-4F8E-8C43-17DE1E07B8ED}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_0ED489CFCE2D5BBE6E7F372033D5229152D9D0AC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{968BD472-8F9A-4242-85C8-467E1034ABD3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="2834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5590" uniqueCount="2834">
   <si>
     <t>snapshot_id</t>
   </si>
@@ -27241,8 +27241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B129" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27350,7 +27350,9 @@
         <v>2020</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="25" t="s">
+        <v>2436</v>
+      </c>
       <c r="J4" t="s">
         <v>643</v>
       </c>
@@ -27378,7 +27380,9 @@
         <v>2020</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="25" t="s">
+        <v>2436</v>
+      </c>
       <c r="J5" t="s">
         <v>643</v>
       </c>
@@ -33441,6 +33445,9 @@
       <c r="G216" s="1">
         <v>2020</v>
       </c>
+      <c r="I216" t="s">
+        <v>2436</v>
+      </c>
       <c r="J216" t="s">
         <v>643</v>
       </c>
@@ -33467,6 +33474,9 @@
       <c r="G217" s="1">
         <v>2020</v>
       </c>
+      <c r="I217" t="s">
+        <v>2436</v>
+      </c>
       <c r="J217" t="s">
         <v>643</v>
       </c>
@@ -33493,6 +33503,9 @@
       <c r="G218" s="1">
         <v>2020</v>
       </c>
+      <c r="I218" t="s">
+        <v>2436</v>
+      </c>
       <c r="J218" t="s">
         <v>643</v>
       </c>
@@ -33519,6 +33532,9 @@
       <c r="G219" s="1">
         <v>2020</v>
       </c>
+      <c r="I219" t="s">
+        <v>2436</v>
+      </c>
       <c r="J219" t="s">
         <v>643</v>
       </c>
@@ -33544,6 +33560,9 @@
       </c>
       <c r="G220" s="1">
         <v>2020</v>
+      </c>
+      <c r="I220" t="s">
+        <v>2436</v>
       </c>
       <c r="J220" t="s">
         <v>643</v>

</xml_diff>